<commit_message>
fixed the standard error
</commit_message>
<xml_diff>
--- a/stroopdata.xlsx
+++ b/stroopdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuaschultz/Desktop/P1 Test a Perceptual Phenomenon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuaschultz/Desktop/Nano Degree/P1 Test a Perceptual Phenomenon/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="stroopdata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Congruent</t>
   </si>
@@ -73,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -117,18 +117,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,11 +412,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090053808"/>
-        <c:axId val="-2090044592"/>
+        <c:axId val="-2110838384"/>
+        <c:axId val="-2133173952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2090053808"/>
+        <c:axId val="-2110838384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,12 +514,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090044592"/>
+        <c:crossAx val="-2133173952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2090044592"/>
+        <c:axId val="-2133173952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,7 +639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090053808"/>
+        <c:crossAx val="-2110838384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1293,13 +1297,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>120650</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -1323,13 +1327,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -1625,23 +1629,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1657,8 +1661,11 @@
       <c r="H1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>12.079000000000001</v>
       </c>
@@ -1677,8 +1684,12 @@
         <f>E2-B2</f>
         <v>7.1989999999999981</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <f>(H2-$B$35)^2</f>
+        <v>0.58643687673611689</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>16.791</v>
       </c>
@@ -1697,8 +1708,12 @@
         <f t="shared" ref="H3:H25" si="2">E3-B3</f>
         <v>1.9499999999999993</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <f t="shared" ref="I3:I25" si="3">(H3-$B$35)^2</f>
+        <v>36.177718793402811</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>9.5640000000000001</v>
       </c>
@@ -1717,8 +1732,12 @@
         <f t="shared" si="2"/>
         <v>11.649999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>13.580760460069421</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>8.6300000000000008</v>
       </c>
@@ -1737,8 +1756,12 @@
         <f t="shared" si="2"/>
         <v>7.0569999999999986</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>0.82408571006945031</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>14.669</v>
       </c>
@@ -1757,8 +1780,12 @@
         <f t="shared" si="2"/>
         <v>8.1340000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>2.8631460069443941E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>12.238</v>
       </c>
@@ -1777,8 +1804,12 @@
         <f t="shared" si="2"/>
         <v>8.64</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>0.45590629340277611</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>14.692</v>
       </c>
@@ -1797,8 +1828,12 @@
         <f t="shared" si="2"/>
         <v>9.879999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>3.6680229600694338</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>8.9870000000000001</v>
       </c>
@@ -1817,8 +1852,12 @@
         <f t="shared" si="2"/>
         <v>8.4069999999999983</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>0.19554821006944129</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>9.4009999999999998</v>
       </c>
@@ -1837,8 +1876,12 @@
         <f t="shared" si="2"/>
         <v>11.361000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>11.53423104340277</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>14.48</v>
       </c>
@@ -1857,8 +1900,12 @@
         <f t="shared" si="2"/>
         <v>11.802</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>14.72416779340276</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>22.327999999999999</v>
       </c>
@@ -1877,8 +1924,12 @@
         <f t="shared" si="2"/>
         <v>2.1960000000000015</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>33.278957293402783</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>15.298</v>
       </c>
@@ -1897,8 +1948,12 @@
         <f t="shared" si="2"/>
         <v>3.3459999999999983</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>21.333236460069475</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>15.073</v>
       </c>
@@ -1917,8 +1972,12 @@
         <f t="shared" si="2"/>
         <v>2.4370000000000012</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>30.556480710069451</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>16.928999999999998</v>
       </c>
@@ -1937,8 +1996,12 @@
         <f t="shared" si="2"/>
         <v>3.4009999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>20.828194376736128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>18.2</v>
       </c>
@@ -1957,8 +2020,12 @@
         <f t="shared" si="2"/>
         <v>17.055000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>82.631887543402797</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>12.13</v>
       </c>
@@ -1977,8 +2044,12 @@
         <f t="shared" si="2"/>
         <v>10.028</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>4.2568286267361053</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>18.495000000000001</v>
       </c>
@@ -1997,8 +2068,12 @@
         <f t="shared" si="2"/>
         <v>6.6439999999999984</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>1.7444906267361202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>10.638999999999999</v>
       </c>
@@ -2017,8 +2092,12 @@
         <f t="shared" si="2"/>
         <v>9.7899999999999991</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>3.3313854600694346</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>11.343999999999999</v>
       </c>
@@ -2037,8 +2116,12 @@
         <f t="shared" si="2"/>
         <v>6.0810000000000013</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>3.5486710434027797</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>12.369</v>
       </c>
@@ -2057,8 +2140,12 @@
         <f t="shared" si="2"/>
         <v>21.918999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>194.71993021006932</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>12.944000000000001</v>
       </c>
@@ -2077,8 +2164,12 @@
         <f t="shared" si="2"/>
         <v>10.949999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>8.9114687934027526</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>14.233000000000001</v>
       </c>
@@ -2097,8 +2188,12 @@
         <f t="shared" si="2"/>
         <v>3.7270000000000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>17.958878210069457</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>19.71</v>
       </c>
@@ -2117,8 +2212,12 @@
         <f t="shared" si="2"/>
         <v>2.347999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>31.548348626736143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>16.004000000000001</v>
       </c>
@@ -2137,8 +2236,12 @@
         <f t="shared" si="2"/>
         <v>5.1529999999999987</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>7.9061723767361292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -2147,7 +2250,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2156,7 +2259,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -2164,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -2186,8 +2289,17 @@
         <v>23.011757036231884</v>
       </c>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H31" s="1">
+        <f>AVERAGE(H2:H25)</f>
+        <v>7.964791666666664</v>
+      </c>
+      <c r="I31" s="1">
+        <f>AVERAGE(I2:I25)</f>
+        <v>22.680434998263888</v>
+      </c>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2204,7 +2316,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -2221,7 +2333,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2229,7 +2341,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -2243,13 +2355,13 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="1">
-        <f>SQRT((C31+F31)/B27)</f>
-        <v>1.2193028422505088</v>
+        <f>I31/SQRT(B27)</f>
+        <v>4.6296244075090005</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2257,7 +2369,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2265,13 +2377,13 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="1">
         <f>B35/B36</f>
-        <v>6.5322505539032303</v>
+        <v>1.7203969405699968</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2279,8 +2391,8 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J46" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L46" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed finishing with the correct calculations and t stat
</commit_message>
<xml_diff>
--- a/stroopdata.xlsx
+++ b/stroopdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="860" windowWidth="21180" windowHeight="15720" tabRatio="500"/>
+    <workbookView xWindow="8080" yWindow="1180" windowWidth="21180" windowHeight="15720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="stroopdata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Congruent</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>T Stat</t>
+  </si>
+  <si>
+    <t>STD of Different</t>
   </si>
 </sst>
 </file>
@@ -117,8 +120,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -128,11 +135,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1629,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2294,8 +2305,8 @@
         <v>7.964791666666664</v>
       </c>
       <c r="I31" s="1">
-        <f>AVERAGE(I2:I25)</f>
-        <v>22.680434998263888</v>
+        <f>SUM(I2:I25)/(COUNT(I2:I25)-1)</f>
+        <v>23.666540867753621</v>
       </c>
       <c r="J31" s="1"/>
     </row>
@@ -2357,11 +2368,11 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B36" s="1">
-        <f>I31/SQRT(B27)</f>
-        <v>4.6296244075090005</v>
+        <f>SQRT(I31)</f>
+        <v>4.8648269103590538</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2370,7 +2381,13 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1">
+        <f>B36/SQRT(B27)</f>
+        <v>0.99302863477834025</v>
+      </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -2378,21 +2395,29 @@
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="1">
-        <f>B35/B36</f>
-        <v>1.7203969405699968</v>
-      </c>
+      <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L46" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="1">
+        <f>B35/B37</f>
+        <v>8.0207069441099623</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L47" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>